<commit_message>
Banco de Dados Finalizado
</commit_message>
<xml_diff>
--- a/Banco de Dados/Modelagens/Modelo-Físico-WTDNWYTK.xlsx
+++ b/Banco de Dados/Modelagens/Modelo-Físico-WTDNWYTK.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25017"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20383"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\48395996888.INFOSCS\Desktop\Projeto_WTDNWYTK\Banco de Dados\Modelagens\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\48395996888.INFOSCS\Documents\Batata\Projeto_WTDNWYTK\Banco de Dados\Modelagens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD71A6EC-6A29-4B4B-80BB-FD242B762F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E52116E-ABC2-456E-9A84-9B4D668DEB8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" firstSheet="3" activeTab="5" xr2:uid="{CFFFCBB5-C331-46BA-9E51-1A3D05742F7D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="3" xr2:uid="{CFFFCBB5-C331-46BA-9E51-1A3D05742F7D}"/>
   </bookViews>
   <sheets>
     <sheet name="usuario" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -330,7 +321,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,9 +449,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -474,6 +462,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -494,7 +485,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -793,26 +784,26 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="A1:D5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -826,7 +817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75">
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -840,7 +831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -854,7 +845,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75">
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -887,22 +878,22 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B11" sqref="B3:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="11"/>
-    </row>
-    <row r="2" spans="1:2" ht="15.75">
+      <c r="B1" s="17"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -910,7 +901,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -918,7 +909,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -926,7 +917,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75">
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -934,7 +925,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -942,7 +933,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75">
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -950,7 +941,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75">
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -958,7 +949,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75">
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -966,7 +957,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75">
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -974,7 +965,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75">
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -982,31 +973,31 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75">
+    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:2" ht="15.75">
+    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:2" ht="15.75">
+    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:2" ht="15.75">
+    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:2" ht="15.75">
+    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="1:2" ht="15.75">
+    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:2" ht="15.75">
+    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
     </row>
@@ -1023,25 +1014,25 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B18" sqref="B3:B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="17"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75">
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -1051,7 +1042,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75">
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1061,7 +1052,7 @@
       <c r="C3" s="8"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1071,7 +1062,7 @@
       <c r="C4" s="8"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75">
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1081,7 +1072,7 @@
       <c r="C5" s="8"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75">
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1089,7 +1080,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75">
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1097,7 +1088,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75">
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1105,7 +1096,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1113,7 +1104,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1121,7 +1112,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75">
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1129,7 +1120,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75">
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1137,7 +1128,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1145,7 +1136,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75">
+    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1153,7 +1144,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75">
+    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1161,7 +1152,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75">
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1169,7 +1160,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75">
+    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1177,7 +1168,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75">
+    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1197,31 +1188,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D853105-6880-4E9D-84BC-E64D86945D95}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="95" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>46</v>
       </c>
@@ -1234,284 +1225,284 @@
       <c r="D2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="96.75">
+    <row r="3" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>1</v>
       </c>
       <c r="B3" s="10">
         <v>1</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-    </row>
-    <row r="4" spans="1:6" ht="32.25">
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>2</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="5" spans="1:6" ht="162">
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="1:6" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>3</v>
       </c>
       <c r="B5" s="10">
         <v>1</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="13"/>
-    </row>
-    <row r="6" spans="1:6" ht="81">
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>4</v>
       </c>
       <c r="B6" s="10">
         <v>1</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="1:6" ht="129">
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="1:6" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>5</v>
       </c>
       <c r="B7" s="10">
         <v>1</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="1:6" ht="291.75">
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="1:6" ht="280.8" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>6</v>
       </c>
       <c r="B8" s="10">
         <v>2</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="1:6" ht="129">
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:6" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>7</v>
       </c>
       <c r="B9" s="10">
         <v>2</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:6" ht="129">
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:6" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>8</v>
       </c>
       <c r="B10" s="10">
         <v>2</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="1:6" ht="210.75">
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>9</v>
       </c>
       <c r="B11" s="10">
         <v>2</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="13"/>
-    </row>
-    <row r="12" spans="1:6" ht="113.25">
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>10</v>
       </c>
       <c r="B12" s="10">
         <v>2</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="1:6" ht="388.5">
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" ht="358.8" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <v>11</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="12">
         <v>3</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="404.25">
+    <row r="14" spans="1:6" ht="390" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>12</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="12">
         <v>3</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="1:6" ht="178.5">
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>13</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="12">
         <v>3</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="1:6" ht="96.75">
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>14</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="12">
         <v>3</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="12" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="129">
+    <row r="17" spans="1:6" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>15</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="12">
         <v>3</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1529,15 +1520,15 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="11"/>
-    </row>
-    <row r="2" spans="1:2" ht="15.75">
+      <c r="B1" s="17"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>46</v>
       </c>
@@ -1545,7 +1536,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1553,7 +1544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1561,7 +1552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75">
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1569,7 +1560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1577,7 +1568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75">
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1585,7 +1576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75">
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1593,7 +1584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75">
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1601,7 +1592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75">
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1609,7 +1600,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75">
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1617,7 +1608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75">
+    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -1625,7 +1616,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75">
+    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -1633,7 +1624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75">
+    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>9</v>
       </c>
@@ -1641,7 +1632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75">
+    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>10</v>
       </c>
@@ -1649,7 +1640,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75">
+    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>10</v>
       </c>
@@ -1657,7 +1648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75">
+    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>11</v>
       </c>
@@ -1665,7 +1656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75">
+    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>12</v>
       </c>
@@ -1673,7 +1664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75">
+    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>12</v>
       </c>
@@ -1681,7 +1672,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75">
+    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>13</v>
       </c>
@@ -1689,7 +1680,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75">
+    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>13</v>
       </c>
@@ -1697,7 +1688,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75">
+    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>13</v>
       </c>
@@ -1705,7 +1696,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75">
+    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>13</v>
       </c>
@@ -1713,7 +1704,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75">
+    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>14</v>
       </c>
@@ -1721,7 +1712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75">
+    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>14</v>
       </c>
@@ -1729,7 +1720,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75">
+    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>14</v>
       </c>
@@ -1737,7 +1728,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75">
+    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>15</v>
       </c>
@@ -1745,7 +1736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75">
+    <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>15</v>
       </c>
@@ -1765,19 +1756,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF760824-4AEF-4AE3-92A5-955D7139F651}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="11"/>
-    </row>
-    <row r="2" spans="1:2" ht="15.75">
+      <c r="B1" s="17"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>46</v>
       </c>
@@ -1785,7 +1776,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1793,7 +1784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1801,7 +1792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75">
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1809,7 +1800,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1817,7 +1808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75">
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1825,7 +1816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75">
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1833,7 +1824,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75">
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1841,7 +1832,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75">
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -1849,7 +1840,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75">
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>6</v>
       </c>
@@ -1857,7 +1848,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75">
+    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>7</v>
       </c>
@@ -1865,7 +1856,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75">
+    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>7</v>
       </c>
@@ -1873,7 +1864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75">
+    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>8</v>
       </c>
@@ -1881,7 +1872,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75">
+    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>9</v>
       </c>
@@ -1889,7 +1880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75">
+    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>9</v>
       </c>
@@ -1897,7 +1888,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75">
+    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>10</v>
       </c>
@@ -1905,7 +1896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75">
+    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>10</v>
       </c>
@@ -1913,7 +1904,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75">
+    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>11</v>
       </c>
@@ -1921,7 +1912,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75">
+    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>11</v>
       </c>
@@ -1929,7 +1920,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75">
+    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>11</v>
       </c>
@@ -1937,7 +1928,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75">
+    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>11</v>
       </c>
@@ -1945,7 +1936,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75">
+    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>11</v>
       </c>
@@ -1953,7 +1944,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75">
+    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>12</v>
       </c>
@@ -1961,7 +1952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75">
+    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>13</v>
       </c>
@@ -1969,7 +1960,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75">
+    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>13</v>
       </c>
@@ -1977,7 +1968,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75">
+    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>14</v>
       </c>
@@ -1985,7 +1976,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75">
+    <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>14</v>
       </c>
@@ -1993,7 +1984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75">
+    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>15</v>
       </c>
@@ -2001,7 +1992,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75">
+    <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>15</v>
       </c>

</xml_diff>